<commit_message>
fixed conceptual error in the model
</commit_message>
<xml_diff>
--- a/tests/models/linear/4_infra_year_timeslices/input_data/input_data.xlsx
+++ b/tests/models/linear/4_infra_year_timeslices/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baioc\Documents\GitHub\pyesm\tests\models\linear\4_infra_year_timeslices\input_data - Copy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baioc\Documents\GitHub\pyesm\tests\models\linear\4_infra_year_timeslices\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E01DC3-53E0-4413-A2CB-89ED69B48134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B64AE0-0E8D-4FA1-8F36-7DC60E67A3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2655" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="u" sheetId="13" r:id="rId1"/>
@@ -125,6 +125,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -471,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51953CA0-7D59-45B5-B653-0A8B392C8438}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1319,7 +1320,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1336,7 +1337,7 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>1500</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1353,7 +1354,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2440,8 +2441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,7 +2478,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>6000</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2494,7 +2495,7 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>8000</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,7 +2512,7 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>2500</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2528,7 +2529,7 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>2500</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2545,7 +2546,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>2500</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2562,7 +2563,7 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <v>2500</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>